<commit_message>
Selection of runs for the grid
</commit_message>
<xml_diff>
--- a/documentation/List of models.xlsx
+++ b/documentation/List of models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Slava\Documents\kineticsim_reader\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4062C2F-C912-4604-9CBF-8C51F1F560E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F07C27B-99E0-4EEF-B8D2-13CD6494A3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -203,7 +203,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -212,9 +212,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -500,7 +497,7 @@
   <dimension ref="B2:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,7 +761,7 @@
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C17" s="2">

</xml_diff>

<commit_message>
VDF 40x40 dataset added
</commit_message>
<xml_diff>
--- a/documentation/List of models.xlsx
+++ b/documentation/List of models.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Slava\Documents\kineticsim_reader\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4AE070F-416D-4383-85BF-5CABC29FD447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF36BA91-613D-4A21-A29B-588DCDE3D3E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="210" yWindow="2865" windowWidth="27855" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -524,7 +524,7 @@
   <dimension ref="B2:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>